<commit_message>
Push to other PC
</commit_message>
<xml_diff>
--- a/Assets/ExampleRapport.xlsx
+++ b/Assets/ExampleRapport.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sharks\Documents\GradWork\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D34A7D-AFBC-40D1-B5D2-EE17A6AA0B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97327E3D-F6C9-40E3-8736-BD23AE730726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="1" r:id="rId1"/>
-    <sheet name="Graphs" sheetId="2" r:id="rId2"/>
+    <sheet name="Calculations for graphs" sheetId="3" r:id="rId2"/>
+    <sheet name="Graphs" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Stats!$A$1:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Stats!$A$1:$F$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,10 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Iteration</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="14">
   <si>
     <t>Puzzle</t>
   </si>
@@ -67,6 +65,24 @@
   </si>
   <si>
     <t>Dummy v.1</t>
+  </si>
+  <si>
+    <t>Depth-First Search v.1</t>
+  </si>
+  <si>
+    <t>success rate</t>
+  </si>
+  <si>
+    <t>average time</t>
+  </si>
+  <si>
+    <t>Suguru</t>
+  </si>
+  <si>
+    <t>Word Search</t>
+  </si>
+  <si>
+    <t>Binary</t>
   </si>
 </sst>
 </file>
@@ -401,23 +417,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A13" sqref="A13:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -436,45 +451,330 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
+      <c r="C2">
         <v>250</v>
       </c>
+      <c r="D2" s="1">
+        <v>44929.852881944447</v>
+      </c>
       <c r="E2" s="1">
-        <v>44929.852881944447</v>
-      </c>
-      <c r="F2" s="1">
         <v>44929.852893518517</v>
       </c>
-      <c r="G2" s="2">
-        <f>F2-E2</f>
+      <c r="F2" s="2">
+        <f>E2-D2</f>
         <v>1.1574069503694773E-5</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>617</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44935.375543981485</v>
+      </c>
+      <c r="E3" s="1">
+        <v>44935.375543981485</v>
+      </c>
+      <c r="F3" s="2">
+        <f>E3-D3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>617</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44935.375567129631</v>
+      </c>
+      <c r="E4" s="1">
+        <v>44935.375567129631</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" ref="F4:F12" si="0">E4-D4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>617</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44935.375567129631</v>
+      </c>
+      <c r="E5" s="1">
+        <v>44935.375578703701</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1574069503694773E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>617</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44935.375578703701</v>
+      </c>
+      <c r="E6" s="1">
+        <v>44935.375578703701</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>617</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44935.375578703701</v>
+      </c>
+      <c r="E7" s="1">
+        <v>44935.375578703701</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>617</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44935.375578703701</v>
+      </c>
+      <c r="E8" s="1">
+        <v>44935.375578703701</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>617</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44935.375578703701</v>
+      </c>
+      <c r="E9" s="1">
+        <v>44935.375578703701</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>617</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44935.375578703701</v>
+      </c>
+      <c r="E10" s="1">
+        <v>44935.375578703701</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>617</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44935.375578703701</v>
+      </c>
+      <c r="E11" s="1">
+        <v>44935.375578703701</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>617</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44935.375578703701</v>
+      </c>
+      <c r="E12" s="1">
+        <v>44935.375578703701</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:F12" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACFD2CD0-2613-4569-88EB-5C15C7A17353}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B13ACC1-2529-422B-8011-EAA40BE09A14}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
DFS v2 + Sudoku Check in puzzle logic
</commit_message>
<xml_diff>
--- a/Assets/ExampleRapport.xlsx
+++ b/Assets/ExampleRapport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sharks\Documents\GradWork\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97327E3D-F6C9-40E3-8736-BD23AE730726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52786EF9-3C75-4C67-859F-E63C0FF1EF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="1" r:id="rId1"/>
@@ -419,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,74 +691,79 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACFD2CD0-2613-4569-88EB-5C15C7A17353}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="2">
+        <f>AVERAGE(Stats!F2:F12)</f>
+        <v>2.1043762733990494E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>10</v>
       </c>

</xml_diff>